<commit_message>
make the excel more beautiful
</commit_message>
<xml_diff>
--- a/bugs.xlsx
+++ b/bugs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="510" yWindow="855" windowWidth="18855" windowHeight="5085"/>
+    <workbookView xWindow="270" yWindow="540" windowWidth="19095" windowHeight="5400"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet0" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>problem_id(改数列没数据整行作废说)</t>
   </si>
@@ -22,6 +22,9 @@
     <t>description</t>
   </si>
   <si>
+    <t>result(未解决(尚未处理)、未解决(延后解决)、未解决(无法解决)、未解决(不需解决)、未解决(无法重现)、解决(修复成功)、解决(不是缺陷)、解决(重复缺陷))</t>
+  </si>
+  <si>
     <t>problemSolution</t>
   </si>
   <si>
@@ -37,23 +40,15 @@
     <t/>
   </si>
   <si>
-    <t>隐藏/browse/HSTZYJF-21170</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>描述</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>result(未解决(尚未处理)、未解决(延后解决)、未解决(无法解决)、未解决(不需解决)、未解决(无法重现)、解决(修复成功)、解决(不是缺陷)、解决(重复缺陷))</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>分配给你</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>某某</t>
+    <t>/dm/browse/HSTZYJF-21170</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>browse/HSTZYJF-21169</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>描述1</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -61,14 +56,23 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>某人</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>什么什么问题</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>解决(修复成功)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>添加修改方案</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>添加备注</t>
+    <t>添加修改备注</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -76,7 +80,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -85,10 +89,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <name val="黑体"/>
-      <family val="3"/>
+      <sz val="11"/>
+      <name val="宋体"/>
       <charset val="134"/>
     </font>
     <font>
@@ -97,6 +99,12 @@
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -107,25 +115,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thick">
-        <color indexed="10"/>
-      </top>
-      <bottom style="double">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -143,71 +138,21 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="thick">
-        <color indexed="10"/>
-      </top>
-      <bottom style="double">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="thick">
-        <color indexed="10"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="22" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
+    <xf numFmtId="22" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="22" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
+    <xf numFmtId="22" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -512,81 +457,88 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="59.875" customWidth="1"/>
-    <col min="2" max="2" width="72.5" customWidth="1"/>
-    <col min="3" max="3" width="24.875" customWidth="1"/>
-    <col min="4" max="4" width="17.75" customWidth="1"/>
-    <col min="5" max="5" width="20.25" customWidth="1"/>
+    <col min="2" max="2" width="39.125" customWidth="1"/>
+    <col min="4" max="4" width="30" customWidth="1"/>
+    <col min="5" max="5" width="28" customWidth="1"/>
+    <col min="7" max="7" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="30" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="30" customHeight="1">
+      <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="30" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="23.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="23.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="14.25" thickTop="1" x14ac:dyDescent="0.15"/>
+    <row r="4" spans="1:7" ht="14.25" thickTop="1"/>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>